<commit_message>
mis pendientes q no he terminado parte 2
</commit_message>
<xml_diff>
--- a/doc/pendientes.xlsx
+++ b/doc/pendientes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="109">
   <si>
     <t>checar nullos en la recreacion y el envio de solicitudes (en la recreacion el servicio no regresa algun campo en este ejemplo ingresos, en la nueva sol, enviar 0)</t>
   </si>
@@ -327,6 +327,33 @@
   </si>
   <si>
     <t>ENVIAR SERVICIOS QUE NO SIRVEN PARA QUE ME LOS ARREGLEN</t>
+  </si>
+  <si>
+    <t>LOAD AGREGARLO ADIV CON EXTENCION MAX</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t>agregar validacion de WS invalid</t>
+  </si>
+  <si>
+    <t>LOADING INDEX DESHABILITANDO EL ACCESAR</t>
+  </si>
+  <si>
+    <t>Agregar nombre a la firma</t>
+  </si>
+  <si>
+    <t>Integrar ocr de CC y Pasaporte</t>
+  </si>
+  <si>
+    <t>se acordo que asi por el momento esta bien Erdnando</t>
+  </si>
+  <si>
+    <t>Erdnando</t>
+  </si>
+  <si>
+    <t>COMENTADO CON ERDNANADO</t>
   </si>
 </sst>
 </file>
@@ -656,11 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +710,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>84</v>
       </c>
@@ -692,7 +718,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>89</v>
       </c>
@@ -700,7 +726,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>90</v>
       </c>
@@ -708,7 +734,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>91</v>
       </c>
@@ -716,7 +742,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -729,13 +755,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C7" s="4">
-        <v>42767</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>43004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -743,7 +769,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -751,7 +777,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -759,7 +785,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -767,7 +793,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -775,7 +801,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -783,7 +809,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -791,7 +817,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -799,7 +825,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -807,7 +833,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -815,18 +841,18 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -845,12 +871,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -869,7 +895,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
@@ -877,7 +903,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -885,7 +911,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
@@ -893,7 +919,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -901,7 +927,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -917,7 +943,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -933,7 +959,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -941,7 +967,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -949,7 +975,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -957,7 +983,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>28</v>
       </c>
@@ -965,7 +991,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -973,15 +999,18 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
@@ -989,7 +1018,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
@@ -997,7 +1026,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
@@ -1005,7 +1034,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -1013,7 +1042,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
@@ -1021,7 +1050,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
@@ -1029,7 +1058,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
@@ -1037,7 +1066,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
@@ -1045,7 +1074,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>39</v>
       </c>
@@ -1053,7 +1082,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1090,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>40</v>
       </c>
@@ -1069,7 +1098,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>41</v>
       </c>
@@ -1077,15 +1106,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>43</v>
       </c>
@@ -1093,7 +1122,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>44</v>
       </c>
@@ -1101,7 +1130,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>45</v>
       </c>
@@ -1109,15 +1138,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>47</v>
       </c>
@@ -1125,7 +1154,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>48</v>
       </c>
@@ -1133,7 +1162,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>49</v>
       </c>
@@ -1141,7 +1170,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>50</v>
       </c>
@@ -1149,15 +1178,18 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>52</v>
       </c>
@@ -1165,7 +1197,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>53</v>
       </c>
@@ -1173,7 +1205,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>54</v>
       </c>
@@ -1181,15 +1213,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>56</v>
       </c>
@@ -1202,7 +1234,7 @@
         <v>57</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1213,7 +1245,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>59</v>
       </c>
@@ -1229,7 +1261,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>61</v>
       </c>
@@ -1237,7 +1269,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>62</v>
       </c>
@@ -1245,7 +1277,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>63</v>
       </c>
@@ -1253,7 +1285,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>64</v>
       </c>
@@ -1261,7 +1293,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>65</v>
       </c>
@@ -1269,7 +1301,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>66</v>
       </c>
@@ -1277,7 +1309,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>67</v>
       </c>
@@ -1285,7 +1317,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>68</v>
       </c>
@@ -1293,7 +1325,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>69</v>
       </c>
@@ -1325,7 +1357,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>73</v>
       </c>
@@ -1333,7 +1365,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>74</v>
       </c>
@@ -1341,7 +1373,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>75</v>
       </c>
@@ -1349,7 +1381,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>76</v>
       </c>
@@ -1357,7 +1389,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>77</v>
       </c>
@@ -1365,7 +1397,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>78</v>
       </c>
@@ -1373,7 +1405,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>79</v>
       </c>
@@ -1381,7 +1413,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>80</v>
       </c>
@@ -1389,7 +1421,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>81</v>
       </c>
@@ -1397,7 +1429,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>82</v>
       </c>
@@ -1405,38 +1437,72 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C91">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Pendiente"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C91"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
MODIFICACION DEL MODAL DE IMAGENES
</commit_message>
<xml_diff>
--- a/doc/pendientes.xlsx
+++ b/doc/pendientes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Omar\Documents\AfiliaMaaSV7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Omar\Documents\proyectos\afiliamaas-web\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="110">
   <si>
     <t>checar nullos en la recreacion y el envio de solicitudes (en la recreacion el servicio no regresa algun campo en este ejemplo ingresos, en la nueva sol, enviar 0)</t>
   </si>
@@ -353,7 +353,10 @@
     <t>Erdnando</t>
   </si>
   <si>
-    <t>COMENTADO CON ERDNANADO</t>
+    <t xml:space="preserve">it </t>
+  </si>
+  <si>
+    <t>CAMBIAR ALERT POR MODAL</t>
   </si>
 </sst>
 </file>
@@ -683,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +844,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>92</v>
       </c>
@@ -1499,6 +1502,11 @@
       </c>
       <c r="B99" s="2" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ACTUALIZACION DE SLASH MENU NUEVA SOLICITUD
</commit_message>
<xml_diff>
--- a/doc/pendientes.xlsx
+++ b/doc/pendientes.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$93</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="118">
   <si>
     <t>checar nullos en la recreacion y el envio de solicitudes (en la recreacion el servicio no regresa algun campo en este ejemplo ingresos, en la nueva sol, enviar 0)</t>
   </si>
@@ -347,9 +347,6 @@
     <t>Integrar ocr de CC y Pasaporte</t>
   </si>
   <si>
-    <t>se acordo que asi por el momento esta bien Erdnando</t>
-  </si>
-  <si>
     <t>Erdnando</t>
   </si>
   <si>
@@ -357,6 +354,33 @@
   </si>
   <si>
     <t>CAMBIAR ALERT POR MODAL</t>
+  </si>
+  <si>
+    <t>ACTUAL 28092017</t>
+  </si>
+  <si>
+    <t>TODO EN MODAL</t>
+  </si>
+  <si>
+    <t>xml ESTÁNDAR 50 MAX LENGTH</t>
+  </si>
+  <si>
+    <t>validacion del lado de los servicios ante una autenticacion incorrectar</t>
+  </si>
+  <si>
+    <t>validar el querystring que se pueda descifrar correctamente y en automatico mandar a ligin indicando que no mame</t>
+  </si>
+  <si>
+    <t>XML</t>
+  </si>
+  <si>
+    <t>versionador funcionando</t>
+  </si>
+  <si>
+    <t>recordar usuario</t>
+  </si>
+  <si>
+    <t>A FUTURO</t>
   </si>
 </sst>
 </file>
@@ -372,12 +396,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -392,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -406,6 +436,13 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +873,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -844,135 +881,119 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>92</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>87</v>
@@ -980,23 +1001,26 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>87</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>87</v>
@@ -1004,74 +1028,74 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>87</v>
@@ -1079,15 +1103,15 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>87</v>
@@ -1095,55 +1119,55 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>87</v>
@@ -1151,7 +1175,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>87</v>
@@ -1159,42 +1183,42 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>87</v>
@@ -1202,23 +1226,23 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>87</v>
@@ -1226,291 +1250,392 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="C79" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="B80" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" s="6"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="7"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="B81" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="6"/>
+      <c r="D81" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="B82" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C82" s="6"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="7"/>
+      <c r="I82" s="7"/>
+      <c r="J82" s="7"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="B83" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83" s="7">
+        <v>1</v>
+      </c>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+    </row>
+    <row r="86" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C86" s="6"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+    </row>
+    <row r="87" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="B88" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C88" s="6"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="B89" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C89" s="6"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
+    </row>
+    <row r="90" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="B90" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="B91" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="B92" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
+      <c r="B93" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="B95" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="B96" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="B100" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>109</v>
+      <c r="B101" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C91"/>
+  <autoFilter ref="A1:C93"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
actualizacion eventos de controles
</commit_message>
<xml_diff>
--- a/doc/pendientes.xlsx
+++ b/doc/pendientes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="141">
   <si>
     <t>checar nullos en la recreacion y el envio de solicitudes (en la recreacion el servicio no regresa algun campo en este ejemplo ingresos, en la nueva sol, enviar 0)</t>
   </si>
@@ -381,6 +381,75 @@
   </si>
   <si>
     <t>A FUTURO</t>
+  </si>
+  <si>
+    <t>AL RECREAR INGRESAR FECHA VALIDA ACTUALMENTE LA DEJA CON FORMATO DE INICIO, VALIDAR COLONIA, NOeXSTERIOR MENOR A 3</t>
+  </si>
+  <si>
+    <t>Deshabilitar el agregar a las imagens de extras</t>
+  </si>
+  <si>
+    <t>REVISAR TOKEN LA EXPIRACIÓN</t>
+  </si>
+  <si>
+    <t>Ocr desahabilitar visivilidad</t>
+  </si>
+  <si>
+    <t>revisar los success de las pantallas de nueva solicitud en los inputs llenados por medio del OCR</t>
+  </si>
+  <si>
+    <t>validar el contenido de los registros regresador por OCR y mostrar o no dependiendo del mismo, quitar las validaciones para eventos de inicio</t>
+  </si>
+  <si>
+    <t>las validaciones d elos campos se dispararán al dar clic sobre los mismos, cambios, blur y al dar clic en siguiente</t>
+  </si>
+  <si>
+    <t>Resetear los controles y validaciones al dar click hacia atrás en header futeer</t>
+  </si>
+  <si>
+    <t>quitar colores a las etiquetas de los validator</t>
+  </si>
+  <si>
+    <t>habilitar spiner con un max de 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revision de correo,  pendejo esto ya estaba </t>
+  </si>
+  <si>
+    <t>validar los telefonos colocar paloma hasta 10 digitos menos de estos colocar amarillo</t>
+  </si>
+  <si>
+    <t>que no se borre el numero de telefono si es menor que 10 en el blur, que no mame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hacer Uppercase en todas las cajas de texto </t>
+  </si>
+  <si>
+    <t>COLOCAR VERDE EN EL HEADER  AL VALIDAR TODO SUCCESS EN EL CLICK ABAJO</t>
+  </si>
+  <si>
+    <t>EN LA PERSONA POLITICA QUITAR CONTENIDO DE inputs si se eleje si y no despues</t>
+  </si>
+  <si>
+    <t>para las referencias familiares validar el llenado de los mismo al meter cualquier campo</t>
+  </si>
+  <si>
+    <t>acomodar el pad de firma</t>
+  </si>
+  <si>
+    <t>validar las imágenes de INE frente atrás y FIRMA como minimo</t>
+  </si>
+  <si>
+    <t>revisar el envio de la solicitud</t>
+  </si>
+  <si>
+    <t>GenerarBitacora de Operaciones</t>
+  </si>
+  <si>
+    <t>modificar la imagen en la presentacion de documentos para que se vea completa</t>
+  </si>
+  <si>
+    <t>Validar si el usuario no ingresa la informacion, click por el header</t>
   </si>
 </sst>
 </file>
@@ -723,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1637,6 +1706,183 @@
         <v>117</v>
       </c>
     </row>
+    <row r="106" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C127" s="6"/>
+    </row>
+    <row r="128" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C93"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
validacion de imagenes regresadas por WS
</commit_message>
<xml_diff>
--- a/doc/pendientes.xlsx
+++ b/doc/pendientes.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$91</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -798,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J127"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,9 +983,25 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>87</v>
@@ -993,7 +1009,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>87</v>
@@ -1001,162 +1017,162 @@
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="A27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>87</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="7"/>
+      <c r="A37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C39" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>87</v>
@@ -1164,15 +1180,15 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>87</v>
@@ -1180,55 +1196,55 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>87</v>
@@ -1236,7 +1252,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>87</v>
@@ -1244,42 +1260,42 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>87</v>
@@ -1287,23 +1303,23 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>87</v>
@@ -1311,34 +1327,34 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C62" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>87</v>
@@ -1346,15 +1362,15 @@
     </row>
     <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>87</v>
@@ -1362,7 +1378,7 @@
     </row>
     <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>87</v>
@@ -1370,15 +1386,15 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>87</v>
@@ -1386,15 +1402,15 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>87</v>
@@ -1402,15 +1418,15 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>87</v>
@@ -1418,50 +1434,68 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>112</v>
-      </c>
+      <c r="A78" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C78" s="6"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>94</v>
@@ -1475,27 +1509,25 @@
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C81" s="6"/>
-      <c r="D81" s="7" t="s">
-        <v>113</v>
+      <c r="C81" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D81" s="7">
+        <v>1</v>
       </c>
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
-      <c r="G81" s="7"/>
-      <c r="H81" s="7"/>
-      <c r="I81" s="7"/>
-      <c r="J81" s="7"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>94</v>
@@ -1504,30 +1536,22 @@
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
-      <c r="H82" s="7"/>
-      <c r="I82" s="7"/>
-      <c r="J82" s="7"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C83" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D83" s="7">
-        <v>1</v>
-      </c>
+      <c r="C83" s="6"/>
+      <c r="D83" s="7"/>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>94</v>
@@ -1537,21 +1561,23 @@
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C85" s="6"/>
+      <c r="C85" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>94</v>
@@ -1561,90 +1587,80 @@
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
     </row>
-    <row r="87" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C87" s="6" t="s">
-        <v>93</v>
-      </c>
+      <c r="C87" s="6"/>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C88" s="6"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="7"/>
-      <c r="F88" s="7"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C89" s="6"/>
-      <c r="D89" s="7"/>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7"/>
-    </row>
-    <row r="90" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>83</v>
+      <c r="C91" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>98</v>
+    </row>
+    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>87</v>
@@ -1652,7 +1668,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>87</v>
@@ -1660,7 +1676,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>87</v>
@@ -1668,160 +1684,160 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="C103" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>141</v>
+        <v>94</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C109" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>87</v>
@@ -1829,23 +1845,23 @@
     </row>
     <row r="119" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>94</v>
@@ -1853,52 +1869,36 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C123" s="6"/>
+    </row>
+    <row r="124" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C125" s="6"/>
-    </row>
-    <row r="126" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+    <row r="125" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
         <v>140</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C93"/>
+  <autoFilter ref="A1:C91"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Nueva presentación login diseño aprovado
</commit_message>
<xml_diff>
--- a/doc/pendientes.xlsx
+++ b/doc/pendientes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="162">
   <si>
     <t>checar nullos en la recreacion y el envio de solicitudes (en la recreacion el servicio no regresa algun campo en este ejemplo ingresos, en la nueva sol, enviar 0)</t>
   </si>
@@ -486,6 +486,33 @@
   </si>
   <si>
     <t>IMPLEMENTAR OFUSCAMIENTO DE CODIGO JS</t>
+  </si>
+  <si>
+    <t>TAB DE FUENTE DE OTROS INGRESOS SE VA A OTROS INGRESOS</t>
+  </si>
+  <si>
+    <t>REDUCIR EL TAMAÑO CUANDO TIENE CLASES</t>
+  </si>
+  <si>
+    <t>REVISAR CLASE DE REFERENCIAS SE PIERDE EL BORDE DE SUCCESS O DE LOS STATUS DEL MISMO</t>
+  </si>
+  <si>
+    <t>HACER EL EXTRA 5</t>
+  </si>
+  <si>
+    <t>REVISAR EL VIVRATO DE ANTIGÜEDAD DE EMPLEO</t>
+  </si>
+  <si>
+    <t>QUITAR EL MODAL DE FONDO AL ENVIO DE LA SOLICITUD</t>
+  </si>
+  <si>
+    <t>QUITAR NACIONALIDAD DE LAS REFERENCIAS</t>
+  </si>
+  <si>
+    <t>REVISAR ANTIGÜEDAD</t>
+  </si>
+  <si>
+    <t>ACOMODAR CLASES</t>
   </si>
 </sst>
 </file>
@@ -828,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J135"/>
+  <dimension ref="A1:J142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,6 +1832,9 @@
       <c r="B110" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="C110" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
@@ -1813,6 +1843,9 @@
       <c r="B111" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="C111" s="2" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
@@ -1975,6 +2008,41 @@
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrección de modales y referencias
</commit_message>
<xml_diff>
--- a/doc/pendientes.xlsx
+++ b/doc/pendientes.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$91</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="162">
   <si>
     <t>checar nullos en la recreacion y el envio de solicitudes (en la recreacion el servicio no regresa algun campo en este ejemplo ingresos, en la nueva sol, enviar 0)</t>
   </si>
@@ -857,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,6 +1982,9 @@
       <c r="A129" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="B129" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
@@ -1997,6 +2000,9 @@
       <c r="A132" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="B132" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="133" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
@@ -2020,11 +2026,17 @@
       <c r="A136" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="B136" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="B137" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="138" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
@@ -2035,10 +2047,16 @@
       <c r="A139" s="1" t="s">
         <v>156</v>
       </c>
+      <c r="B139" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>157</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
VALIDACION TELEFONO A 16
</commit_message>
<xml_diff>
--- a/doc/pendientes.xlsx
+++ b/doc/pendientes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="181">
   <si>
     <t>checar nullos en la recreacion y el envio de solicitudes (en la recreacion el servicio no regresa algun campo en este ejemplo ingresos, en la nueva sol, enviar 0)</t>
   </si>
@@ -555,6 +555,21 @@
   </si>
   <si>
     <t>enviar propuesta para tamños y resoluciones</t>
+  </si>
+  <si>
+    <t>OMITIR TAGS EN CASO DE NO CONTENER VALOR</t>
+  </si>
+  <si>
+    <t>Validar caducidad del token</t>
+  </si>
+  <si>
+    <t>agregar el codigo de la validacion de las referencias</t>
+  </si>
+  <si>
+    <t>validacion de telefono diferente</t>
+  </si>
+  <si>
+    <t>Loadin al acomodar las solicitudes</t>
   </si>
 </sst>
 </file>
@@ -604,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -639,6 +654,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J154"/>
+  <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,7 +1945,7 @@
         <v>123</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -2065,7 +2083,7 @@
         <v>171</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -2081,7 +2099,7 @@
         <v>141</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2231,7 +2249,7 @@
         <v>162</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -2270,7 +2288,43 @@
       <c r="A154" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B154" s="12"/>
+      <c r="B154" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C89"/>

</xml_diff>

<commit_message>
nuevo stilo de captura
</commit_message>
<xml_diff>
--- a/doc/pendientes.xlsx
+++ b/doc/pendientes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="181">
   <si>
     <t>checar nullos en la recreacion y el envio de solicitudes (en la recreacion el servicio no regresa algun campo en este ejemplo ingresos, en la nueva sol, enviar 0)</t>
   </si>
@@ -2099,7 +2099,7 @@
         <v>141</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2304,6 +2304,9 @@
       <c r="A156" s="1" t="s">
         <v>177</v>
       </c>
+      <c r="B156" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
@@ -2316,6 +2319,9 @@
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>179</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>